<commit_message>
added more info on articles
</commit_message>
<xml_diff>
--- a/Ng Lab Hallucinations Research Articles.xlsx
+++ b/Ng Lab Hallucinations Research Articles.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Title</t>
   </si>
@@ -92,6 +92,19 @@
   </si>
   <si>
     <t>Unpublished, but has some ideas for future research</t>
+  </si>
+  <si>
+    <t>Detecting hallucinations in large language
+models using semantic entropy</t>
+  </si>
+  <si>
+    <t>Sebastian Farquhar, Jannik Kossen, Lorenz Kuhn, Yarin Gal</t>
+  </si>
+  <si>
+    <t>19 June 2024</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41586-024-07421-0</t>
   </si>
 </sst>
 </file>
@@ -658,10 +671,18 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
@@ -30455,7 +30476,8 @@
     <hyperlink r:id="rId4" ref="D5"/>
     <hyperlink r:id="rId5" ref="D6"/>
     <hyperlink r:id="rId6" ref="D7"/>
+    <hyperlink r:id="rId7" ref="D8"/>
   </hyperlinks>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>